<commit_message>
partial cleaning up of yok yee's code
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
Partially done value mismatch checking for Income taxes (a)
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
updated upload, tempreal, nextpage
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
Edited yy's number of directors
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
check for "" in director field
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
Completed - Checking of values for Trade and other payables
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.88671875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.85546875" style="1"/>
+    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.88671875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.85546875" style="1"/>
+    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.88671875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.85546875" style="1"/>
+    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.88671875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.85546875" style="1"/>
+    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.88671875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.85546875" style="1"/>
+    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.88671875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.85546875" style="1"/>
+    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.88671875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.85546875" style="1"/>
+    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.88671875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.85546875" style="1"/>
+    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.88671875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.85546875" style="1"/>
+    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.88671875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.85546875" style="1"/>
+    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.88671875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.85546875" style="1"/>
+    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.88671875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.85546875" style="1"/>
+    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.88671875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.85546875" style="1"/>
+    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.88671875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.85546875" style="1"/>
+    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.88671875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.85546875" style="1"/>
+    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.88671875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.85546875" style="1"/>
+    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.88671875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.85546875" style="1"/>
+    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.88671875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.85546875" style="1"/>
+    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.88671875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.85546875" style="1"/>
+    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.88671875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.85546875" style="1"/>
+    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.88671875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.85546875" style="1"/>
+    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.88671875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.85546875" style="1"/>
+    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.88671875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.85546875" style="1"/>
+    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.88671875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.85546875" style="1"/>
+    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.88671875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.85546875" style="1"/>
+    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.88671875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.85546875" style="1"/>
+    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.88671875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.85546875" style="1"/>
+    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.88671875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.85546875" style="1"/>
+    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.88671875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.85546875" style="1"/>
+    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.88671875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.85546875" style="1"/>
+    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.88671875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.85546875" style="1"/>
+    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.88671875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.85546875" style="1"/>
+    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.88671875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.85546875" style="1"/>
+    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.88671875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.85546875" style="1"/>
+    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.88671875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.85546875" style="1"/>
+    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.88671875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.85546875" style="1"/>
+    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.88671875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.85546875" style="1"/>
+    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.88671875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.85546875" style="1"/>
+    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.88671875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.85546875" style="1"/>
+    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.88671875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.85546875" style="1"/>
+    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.88671875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.85546875" style="1"/>
+    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.88671875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.85546875" style="1"/>
+    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.88671875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.85546875" style="1"/>
+    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.88671875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.85546875" style="1"/>
+    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.88671875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.85546875" style="1"/>
+    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.88671875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.85546875" style="1"/>
+    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.88671875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.85546875" style="1"/>
+    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.88671875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.85546875" style="1"/>
+    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.88671875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.85546875" style="1"/>
+    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.88671875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.85546875" style="1"/>
+    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.88671875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.85546875" style="1"/>
+    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.88671875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.85546875" style="1"/>
+    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.88671875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.85546875" style="1"/>
+    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.88671875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.85546875" style="1"/>
+    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.88671875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.85546875" style="1"/>
+    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.88671875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.85546875" style="1"/>
+    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.88671875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.85546875" style="1"/>
+    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.88671875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.85546875" style="1"/>
+    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.88671875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.85546875" style="1"/>
+    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.88671875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.85546875" style="1"/>
+    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.88671875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.85546875" style="1"/>
+    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.88671875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.85546875" style="1"/>
+    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.88671875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.85546875" style="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>

<commit_message>
Sub categories are now detected, phoebe please assist to create the form for updating categories
</commit_message>
<xml_diff>
--- a/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
+++ b/pages/report_fs/uploads/VSIG - (Trial Balance).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\ACCOUNTING_TAX\Wen Ai\FS Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weeko\Documents\ITP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BCDF41C0-6592-4C3A-8B8B-EBC9B5CD562F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AC321-A180-431D-84D2-104E3D5ADB02}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{86201A01-D0C0-4A9C-B214-947686C82C91}"/>
   </bookViews>
   <sheets>
     <sheet name="TB 2016" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'TB 2016'!$A$1:$I$71</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -354,10 +354,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]dd/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]dd/mmm/yy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -576,44 +576,44 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -622,62 +622,62 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,123 +686,123 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="14" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="16" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,22 +811,22 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,49 +835,49 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1201,404 +1201,404 @@
   </sheetPr>
   <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G32" activeCellId="3" sqref="G31 G28 G27 G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="10" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -1608,7 +1608,7 @@
       <c r="G1" s="67"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1620,7 +1620,7 @@
       <c r="G2" s="61"/>
       <c r="H2" s="46"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="60"/>
       <c r="C3" s="60"/>
@@ -1632,7 +1632,7 @@
       <c r="G3" s="57"/>
       <c r="H3" s="46"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="60"/>
       <c r="C4" s="60"/>
@@ -1644,7 +1644,7 @@
       <c r="G4" s="57"/>
       <c r="H4" s="46"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="60"/>
       <c r="C5" s="60"/>
@@ -1656,7 +1656,7 @@
       <c r="G5" s="57"/>
       <c r="H5" s="46"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
       <c r="B6" s="60"/>
       <c r="C6" s="60"/>
@@ -1668,7 +1668,7 @@
       <c r="G6" s="57"/>
       <c r="H6" s="46"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -1680,7 +1680,7 @@
       <c r="G7" s="55"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -1702,7 +1702,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45"/>
       <c r="B10" s="44" t="s">
         <v>0</v>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>0</v>
@@ -1775,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="24" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="15"/>
     </row>
-    <row r="71" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="14"/>
       <c r="C71" s="13"/>
       <c r="D71" s="12"/>
@@ -2766,10 +2766,10 @@
       <c r="F71" s="10"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="2:8" ht="12" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -2777,7 +2777,7 @@
       <c r="F73"/>
       <c r="G73"/>
     </row>
-    <row r="74" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
@@ -2785,7 +2785,7 @@
       <c r="F74"/>
       <c r="G74"/>
     </row>
-    <row r="75" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
@@ -2793,7 +2793,7 @@
       <c r="F75"/>
       <c r="G75"/>
     </row>
-    <row r="76" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76" s="7"/>
@@ -2801,7 +2801,7 @@
       <c r="F76" s="7"/>
       <c r="G76"/>
     </row>
-    <row r="77" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77" s="7"/>
@@ -2809,7 +2809,7 @@
       <c r="F77" s="7"/>
       <c r="G77"/>
     </row>
-    <row r="78" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
@@ -2817,7 +2817,7 @@
       <c r="F78"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
@@ -2825,7 +2825,7 @@
       <c r="F79" s="7"/>
       <c r="G79"/>
     </row>
-    <row r="80" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80" s="7"/>
@@ -2833,7 +2833,7 @@
       <c r="F80" s="7"/>
       <c r="G80"/>
     </row>
-    <row r="81" spans="2:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
@@ -2853,403 +2853,403 @@
   </sheetPr>
   <dimension ref="A1:AA68"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="121" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" style="126" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="12.6640625" style="1" customWidth="1"/>
-    <col min="18" max="256" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="4.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="121" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="126" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="8.85546875" style="1"/>
     <col min="257" max="257" width="4" style="1" customWidth="1"/>
-    <col min="258" max="258" width="15.6640625" style="1" customWidth="1"/>
-    <col min="259" max="259" width="25.6640625" style="1" customWidth="1"/>
-    <col min="260" max="263" width="14.6640625" style="1" customWidth="1"/>
-    <col min="264" max="273" width="12.6640625" style="1" customWidth="1"/>
-    <col min="274" max="512" width="8.88671875" style="1"/>
+    <col min="258" max="258" width="15.7109375" style="1" customWidth="1"/>
+    <col min="259" max="259" width="25.7109375" style="1" customWidth="1"/>
+    <col min="260" max="263" width="14.7109375" style="1" customWidth="1"/>
+    <col min="264" max="273" width="12.7109375" style="1" customWidth="1"/>
+    <col min="274" max="512" width="8.85546875" style="1"/>
     <col min="513" max="513" width="4" style="1" customWidth="1"/>
-    <col min="514" max="514" width="15.6640625" style="1" customWidth="1"/>
-    <col min="515" max="515" width="25.6640625" style="1" customWidth="1"/>
-    <col min="516" max="519" width="14.6640625" style="1" customWidth="1"/>
-    <col min="520" max="529" width="12.6640625" style="1" customWidth="1"/>
-    <col min="530" max="768" width="8.88671875" style="1"/>
+    <col min="514" max="514" width="15.7109375" style="1" customWidth="1"/>
+    <col min="515" max="515" width="25.7109375" style="1" customWidth="1"/>
+    <col min="516" max="519" width="14.7109375" style="1" customWidth="1"/>
+    <col min="520" max="529" width="12.7109375" style="1" customWidth="1"/>
+    <col min="530" max="768" width="8.85546875" style="1"/>
     <col min="769" max="769" width="4" style="1" customWidth="1"/>
-    <col min="770" max="770" width="15.6640625" style="1" customWidth="1"/>
-    <col min="771" max="771" width="25.6640625" style="1" customWidth="1"/>
-    <col min="772" max="775" width="14.6640625" style="1" customWidth="1"/>
-    <col min="776" max="785" width="12.6640625" style="1" customWidth="1"/>
-    <col min="786" max="1024" width="8.88671875" style="1"/>
+    <col min="770" max="770" width="15.7109375" style="1" customWidth="1"/>
+    <col min="771" max="771" width="25.7109375" style="1" customWidth="1"/>
+    <col min="772" max="775" width="14.7109375" style="1" customWidth="1"/>
+    <col min="776" max="785" width="12.7109375" style="1" customWidth="1"/>
+    <col min="786" max="1024" width="8.85546875" style="1"/>
     <col min="1025" max="1025" width="4" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="1031" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1032" max="1041" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1042" max="1280" width="8.88671875" style="1"/>
+    <col min="1026" max="1026" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1028" max="1031" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1032" max="1041" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1042" max="1280" width="8.85546875" style="1"/>
     <col min="1281" max="1281" width="4" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1284" max="1287" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1288" max="1297" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1298" max="1536" width="8.88671875" style="1"/>
+    <col min="1282" max="1282" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1283" max="1283" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1284" max="1287" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1288" max="1297" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1298" max="1536" width="8.85546875" style="1"/>
     <col min="1537" max="1537" width="4" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1540" max="1543" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1544" max="1553" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1554" max="1792" width="8.88671875" style="1"/>
+    <col min="1538" max="1538" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1539" max="1539" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1540" max="1543" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1544" max="1553" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1554" max="1792" width="8.85546875" style="1"/>
     <col min="1793" max="1793" width="4" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="15.6640625" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="25.6640625" style="1" customWidth="1"/>
-    <col min="1796" max="1799" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1800" max="1809" width="12.6640625" style="1" customWidth="1"/>
-    <col min="1810" max="2048" width="8.88671875" style="1"/>
+    <col min="1794" max="1794" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1795" max="1795" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1796" max="1799" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1800" max="1809" width="12.7109375" style="1" customWidth="1"/>
+    <col min="1810" max="2048" width="8.85546875" style="1"/>
     <col min="2049" max="2049" width="4" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2052" max="2055" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2056" max="2065" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2066" max="2304" width="8.88671875" style="1"/>
+    <col min="2050" max="2050" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2051" max="2051" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2052" max="2055" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2056" max="2065" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2066" max="2304" width="8.85546875" style="1"/>
     <col min="2305" max="2305" width="4" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2308" max="2311" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2312" max="2321" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2322" max="2560" width="8.88671875" style="1"/>
+    <col min="2306" max="2306" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2307" max="2307" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2308" max="2311" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2312" max="2321" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2322" max="2560" width="8.85546875" style="1"/>
     <col min="2561" max="2561" width="4" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2564" max="2567" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2568" max="2577" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2578" max="2816" width="8.88671875" style="1"/>
+    <col min="2562" max="2562" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2563" max="2563" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2564" max="2567" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2568" max="2577" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2578" max="2816" width="8.85546875" style="1"/>
     <col min="2817" max="2817" width="4" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2820" max="2823" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2824" max="2833" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2834" max="3072" width="8.88671875" style="1"/>
+    <col min="2818" max="2818" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2819" max="2819" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2820" max="2823" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2824" max="2833" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2834" max="3072" width="8.85546875" style="1"/>
     <col min="3073" max="3073" width="4" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3076" max="3079" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3080" max="3089" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3090" max="3328" width="8.88671875" style="1"/>
+    <col min="3074" max="3074" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3075" max="3075" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3076" max="3079" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3080" max="3089" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3090" max="3328" width="8.85546875" style="1"/>
     <col min="3329" max="3329" width="4" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3332" max="3335" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3336" max="3345" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3346" max="3584" width="8.88671875" style="1"/>
+    <col min="3330" max="3330" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3331" max="3331" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3332" max="3335" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3336" max="3345" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3346" max="3584" width="8.85546875" style="1"/>
     <col min="3585" max="3585" width="4" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3588" max="3591" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3592" max="3601" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3602" max="3840" width="8.88671875" style="1"/>
+    <col min="3586" max="3586" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3587" max="3587" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3588" max="3591" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3592" max="3601" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3602" max="3840" width="8.85546875" style="1"/>
     <col min="3841" max="3841" width="4" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="15.6640625" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="25.6640625" style="1" customWidth="1"/>
-    <col min="3844" max="3847" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3848" max="3857" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3858" max="4096" width="8.88671875" style="1"/>
+    <col min="3842" max="3842" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3843" max="3843" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3844" max="3847" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3848" max="3857" width="12.7109375" style="1" customWidth="1"/>
+    <col min="3858" max="4096" width="8.85546875" style="1"/>
     <col min="4097" max="4097" width="4" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4100" max="4103" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4104" max="4113" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4114" max="4352" width="8.88671875" style="1"/>
+    <col min="4098" max="4098" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4099" max="4099" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4100" max="4103" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4104" max="4113" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4114" max="4352" width="8.85546875" style="1"/>
     <col min="4353" max="4353" width="4" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4356" max="4359" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4360" max="4369" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4370" max="4608" width="8.88671875" style="1"/>
+    <col min="4354" max="4354" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4355" max="4355" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4356" max="4359" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4360" max="4369" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4370" max="4608" width="8.85546875" style="1"/>
     <col min="4609" max="4609" width="4" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4612" max="4615" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4616" max="4625" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4626" max="4864" width="8.88671875" style="1"/>
+    <col min="4610" max="4610" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4611" max="4611" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4612" max="4615" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4616" max="4625" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4626" max="4864" width="8.85546875" style="1"/>
     <col min="4865" max="4865" width="4" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4868" max="4871" width="14.6640625" style="1" customWidth="1"/>
-    <col min="4872" max="4881" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4882" max="5120" width="8.88671875" style="1"/>
+    <col min="4866" max="4866" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4867" max="4867" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4868" max="4871" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4872" max="4881" width="12.7109375" style="1" customWidth="1"/>
+    <col min="4882" max="5120" width="8.85546875" style="1"/>
     <col min="5121" max="5121" width="4" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5124" max="5127" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5128" max="5137" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5138" max="5376" width="8.88671875" style="1"/>
+    <col min="5122" max="5122" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5123" max="5123" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5124" max="5127" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5128" max="5137" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5138" max="5376" width="8.85546875" style="1"/>
     <col min="5377" max="5377" width="4" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5380" max="5383" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5384" max="5393" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5394" max="5632" width="8.88671875" style="1"/>
+    <col min="5378" max="5378" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5379" max="5379" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5380" max="5383" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5384" max="5393" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5394" max="5632" width="8.85546875" style="1"/>
     <col min="5633" max="5633" width="4" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5636" max="5639" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5640" max="5649" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5650" max="5888" width="8.88671875" style="1"/>
+    <col min="5634" max="5634" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5635" max="5635" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5636" max="5639" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5640" max="5649" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5650" max="5888" width="8.85546875" style="1"/>
     <col min="5889" max="5889" width="4" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="15.6640625" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="25.6640625" style="1" customWidth="1"/>
-    <col min="5892" max="5895" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5896" max="5905" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5906" max="6144" width="8.88671875" style="1"/>
+    <col min="5890" max="5890" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5891" max="5891" width="25.7109375" style="1" customWidth="1"/>
+    <col min="5892" max="5895" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5896" max="5905" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5906" max="6144" width="8.85546875" style="1"/>
     <col min="6145" max="6145" width="4" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6148" max="6151" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6152" max="6161" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6162" max="6400" width="8.88671875" style="1"/>
+    <col min="6146" max="6146" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6147" max="6147" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6148" max="6151" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6152" max="6161" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6162" max="6400" width="8.85546875" style="1"/>
     <col min="6401" max="6401" width="4" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6404" max="6407" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6408" max="6417" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6418" max="6656" width="8.88671875" style="1"/>
+    <col min="6402" max="6402" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6403" max="6403" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6404" max="6407" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6408" max="6417" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6418" max="6656" width="8.85546875" style="1"/>
     <col min="6657" max="6657" width="4" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6660" max="6663" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6664" max="6673" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6674" max="6912" width="8.88671875" style="1"/>
+    <col min="6658" max="6658" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6659" max="6659" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6660" max="6663" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6664" max="6673" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6674" max="6912" width="8.85546875" style="1"/>
     <col min="6913" max="6913" width="4" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6916" max="6919" width="14.6640625" style="1" customWidth="1"/>
-    <col min="6920" max="6929" width="12.6640625" style="1" customWidth="1"/>
-    <col min="6930" max="7168" width="8.88671875" style="1"/>
+    <col min="6914" max="6914" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6915" max="6915" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6916" max="6919" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6920" max="6929" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6930" max="7168" width="8.85546875" style="1"/>
     <col min="7169" max="7169" width="4" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7172" max="7175" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7176" max="7185" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7186" max="7424" width="8.88671875" style="1"/>
+    <col min="7170" max="7170" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7171" max="7171" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7172" max="7175" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7176" max="7185" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7186" max="7424" width="8.85546875" style="1"/>
     <col min="7425" max="7425" width="4" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7428" max="7431" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7432" max="7441" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7442" max="7680" width="8.88671875" style="1"/>
+    <col min="7426" max="7426" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7427" max="7427" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7428" max="7431" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7432" max="7441" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7442" max="7680" width="8.85546875" style="1"/>
     <col min="7681" max="7681" width="4" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7684" max="7687" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7688" max="7697" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7698" max="7936" width="8.88671875" style="1"/>
+    <col min="7682" max="7682" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7683" max="7683" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7684" max="7687" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7688" max="7697" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7698" max="7936" width="8.85546875" style="1"/>
     <col min="7937" max="7937" width="4" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7940" max="7943" width="14.6640625" style="1" customWidth="1"/>
-    <col min="7944" max="7953" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7954" max="8192" width="8.88671875" style="1"/>
+    <col min="7938" max="7938" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7939" max="7939" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7940" max="7943" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7944" max="7953" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7954" max="8192" width="8.85546875" style="1"/>
     <col min="8193" max="8193" width="4" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8196" max="8199" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8200" max="8209" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8210" max="8448" width="8.88671875" style="1"/>
+    <col min="8194" max="8194" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8195" max="8195" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8196" max="8199" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8200" max="8209" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8210" max="8448" width="8.85546875" style="1"/>
     <col min="8449" max="8449" width="4" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8452" max="8455" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8456" max="8465" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8466" max="8704" width="8.88671875" style="1"/>
+    <col min="8450" max="8450" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8451" max="8451" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8452" max="8455" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8456" max="8465" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8466" max="8704" width="8.85546875" style="1"/>
     <col min="8705" max="8705" width="4" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8708" max="8711" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8712" max="8721" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8722" max="8960" width="8.88671875" style="1"/>
+    <col min="8706" max="8706" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8707" max="8707" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8708" max="8711" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8712" max="8721" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8722" max="8960" width="8.85546875" style="1"/>
     <col min="8961" max="8961" width="4" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="15.6640625" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8964" max="8967" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8968" max="8977" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8978" max="9216" width="8.88671875" style="1"/>
+    <col min="8962" max="8962" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8963" max="8963" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8964" max="8967" width="14.7109375" style="1" customWidth="1"/>
+    <col min="8968" max="8977" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8978" max="9216" width="8.85546875" style="1"/>
     <col min="9217" max="9217" width="4" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9220" max="9223" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9224" max="9233" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9234" max="9472" width="8.88671875" style="1"/>
+    <col min="9218" max="9218" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9219" max="9219" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9220" max="9223" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9224" max="9233" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9234" max="9472" width="8.85546875" style="1"/>
     <col min="9473" max="9473" width="4" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9476" max="9479" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9480" max="9489" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9490" max="9728" width="8.88671875" style="1"/>
+    <col min="9474" max="9474" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9475" max="9475" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9476" max="9479" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9480" max="9489" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9490" max="9728" width="8.85546875" style="1"/>
     <col min="9729" max="9729" width="4" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9732" max="9735" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9736" max="9745" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9746" max="9984" width="8.88671875" style="1"/>
+    <col min="9730" max="9730" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9731" max="9731" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9732" max="9735" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9736" max="9745" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9746" max="9984" width="8.85546875" style="1"/>
     <col min="9985" max="9985" width="4" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="15.6640625" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="25.6640625" style="1" customWidth="1"/>
-    <col min="9988" max="9991" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9992" max="10001" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10002" max="10240" width="8.88671875" style="1"/>
+    <col min="9986" max="9986" width="15.7109375" style="1" customWidth="1"/>
+    <col min="9987" max="9987" width="25.7109375" style="1" customWidth="1"/>
+    <col min="9988" max="9991" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9992" max="10001" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10002" max="10240" width="8.85546875" style="1"/>
     <col min="10241" max="10241" width="4" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10244" max="10247" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10248" max="10257" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10258" max="10496" width="8.88671875" style="1"/>
+    <col min="10242" max="10242" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10243" max="10243" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10244" max="10247" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10248" max="10257" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10258" max="10496" width="8.85546875" style="1"/>
     <col min="10497" max="10497" width="4" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10500" max="10503" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10504" max="10513" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10514" max="10752" width="8.88671875" style="1"/>
+    <col min="10498" max="10498" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10499" max="10499" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10500" max="10503" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10504" max="10513" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10514" max="10752" width="8.85546875" style="1"/>
     <col min="10753" max="10753" width="4" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10756" max="10759" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10760" max="10769" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10770" max="11008" width="8.88671875" style="1"/>
+    <col min="10754" max="10754" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10755" max="10755" width="25.7109375" style="1" customWidth="1"/>
+    <col min="10756" max="10759" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10760" max="10769" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10770" max="11008" width="8.85546875" style="1"/>
     <col min="11009" max="11009" width="4" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11012" max="11015" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11016" max="11025" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11026" max="11264" width="8.88671875" style="1"/>
+    <col min="11010" max="11010" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11011" max="11011" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11012" max="11015" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11016" max="11025" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11026" max="11264" width="8.85546875" style="1"/>
     <col min="11265" max="11265" width="4" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11268" max="11271" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11272" max="11281" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11282" max="11520" width="8.88671875" style="1"/>
+    <col min="11266" max="11266" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11267" max="11267" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11268" max="11271" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11272" max="11281" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11282" max="11520" width="8.85546875" style="1"/>
     <col min="11521" max="11521" width="4" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11524" max="11527" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11528" max="11537" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11538" max="11776" width="8.88671875" style="1"/>
+    <col min="11522" max="11522" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11523" max="11523" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11524" max="11527" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11528" max="11537" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11538" max="11776" width="8.85546875" style="1"/>
     <col min="11777" max="11777" width="4" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="25.6640625" style="1" customWidth="1"/>
-    <col min="11780" max="11783" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11784" max="11793" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11794" max="12032" width="8.88671875" style="1"/>
+    <col min="11778" max="11778" width="15.7109375" style="1" customWidth="1"/>
+    <col min="11779" max="11779" width="25.7109375" style="1" customWidth="1"/>
+    <col min="11780" max="11783" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11784" max="11793" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11794" max="12032" width="8.85546875" style="1"/>
     <col min="12033" max="12033" width="4" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12036" max="12039" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12040" max="12049" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12050" max="12288" width="8.88671875" style="1"/>
+    <col min="12034" max="12034" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12035" max="12035" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12036" max="12039" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12040" max="12049" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12050" max="12288" width="8.85546875" style="1"/>
     <col min="12289" max="12289" width="4" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12292" max="12295" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12296" max="12305" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12306" max="12544" width="8.88671875" style="1"/>
+    <col min="12290" max="12290" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12291" max="12291" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12292" max="12295" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12296" max="12305" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12306" max="12544" width="8.85546875" style="1"/>
     <col min="12545" max="12545" width="4" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12548" max="12551" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12552" max="12561" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12562" max="12800" width="8.88671875" style="1"/>
+    <col min="12546" max="12546" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12547" max="12547" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12548" max="12551" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12552" max="12561" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12562" max="12800" width="8.85546875" style="1"/>
     <col min="12801" max="12801" width="4" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="15.6640625" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="25.6640625" style="1" customWidth="1"/>
-    <col min="12804" max="12807" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12808" max="12817" width="12.6640625" style="1" customWidth="1"/>
-    <col min="12818" max="13056" width="8.88671875" style="1"/>
+    <col min="12802" max="12802" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12803" max="12803" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12804" max="12807" width="14.7109375" style="1" customWidth="1"/>
+    <col min="12808" max="12817" width="12.7109375" style="1" customWidth="1"/>
+    <col min="12818" max="13056" width="8.85546875" style="1"/>
     <col min="13057" max="13057" width="4" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13060" max="13063" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13064" max="13073" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13074" max="13312" width="8.88671875" style="1"/>
+    <col min="13058" max="13058" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13059" max="13059" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13060" max="13063" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13064" max="13073" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13074" max="13312" width="8.85546875" style="1"/>
     <col min="13313" max="13313" width="4" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13316" max="13319" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13320" max="13329" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13330" max="13568" width="8.88671875" style="1"/>
+    <col min="13314" max="13314" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13315" max="13315" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13316" max="13319" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13320" max="13329" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13330" max="13568" width="8.85546875" style="1"/>
     <col min="13569" max="13569" width="4" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13572" max="13575" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13576" max="13585" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13586" max="13824" width="8.88671875" style="1"/>
+    <col min="13570" max="13570" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13571" max="13571" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13572" max="13575" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13576" max="13585" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13586" max="13824" width="8.85546875" style="1"/>
     <col min="13825" max="13825" width="4" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="15.6640625" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="25.6640625" style="1" customWidth="1"/>
-    <col min="13828" max="13831" width="14.6640625" style="1" customWidth="1"/>
-    <col min="13832" max="13841" width="12.6640625" style="1" customWidth="1"/>
-    <col min="13842" max="14080" width="8.88671875" style="1"/>
+    <col min="13826" max="13826" width="15.7109375" style="1" customWidth="1"/>
+    <col min="13827" max="13827" width="25.7109375" style="1" customWidth="1"/>
+    <col min="13828" max="13831" width="14.7109375" style="1" customWidth="1"/>
+    <col min="13832" max="13841" width="12.7109375" style="1" customWidth="1"/>
+    <col min="13842" max="14080" width="8.85546875" style="1"/>
     <col min="14081" max="14081" width="4" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14084" max="14087" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14088" max="14097" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14098" max="14336" width="8.88671875" style="1"/>
+    <col min="14082" max="14082" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14083" max="14083" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14084" max="14087" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14088" max="14097" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14098" max="14336" width="8.85546875" style="1"/>
     <col min="14337" max="14337" width="4" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14340" max="14343" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14344" max="14353" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14354" max="14592" width="8.88671875" style="1"/>
+    <col min="14338" max="14338" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14339" max="14339" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14340" max="14343" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14344" max="14353" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14354" max="14592" width="8.85546875" style="1"/>
     <col min="14593" max="14593" width="4" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14596" max="14599" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14600" max="14609" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14610" max="14848" width="8.88671875" style="1"/>
+    <col min="14594" max="14594" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14595" max="14595" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14596" max="14599" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14600" max="14609" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14610" max="14848" width="8.85546875" style="1"/>
     <col min="14849" max="14849" width="4" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="25.6640625" style="1" customWidth="1"/>
-    <col min="14852" max="14855" width="14.6640625" style="1" customWidth="1"/>
-    <col min="14856" max="14865" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14866" max="15104" width="8.88671875" style="1"/>
+    <col min="14850" max="14850" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14851" max="14851" width="25.7109375" style="1" customWidth="1"/>
+    <col min="14852" max="14855" width="14.7109375" style="1" customWidth="1"/>
+    <col min="14856" max="14865" width="12.7109375" style="1" customWidth="1"/>
+    <col min="14866" max="15104" width="8.85546875" style="1"/>
     <col min="15105" max="15105" width="4" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15108" max="15111" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15112" max="15121" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15122" max="15360" width="8.88671875" style="1"/>
+    <col min="15106" max="15106" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15107" max="15107" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15108" max="15111" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15112" max="15121" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15122" max="15360" width="8.85546875" style="1"/>
     <col min="15361" max="15361" width="4" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15364" max="15367" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15368" max="15377" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15378" max="15616" width="8.88671875" style="1"/>
+    <col min="15362" max="15362" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15363" max="15363" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15364" max="15367" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15368" max="15377" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15378" max="15616" width="8.85546875" style="1"/>
     <col min="15617" max="15617" width="4" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15620" max="15623" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15624" max="15633" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15634" max="15872" width="8.88671875" style="1"/>
+    <col min="15618" max="15618" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15619" max="15619" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15620" max="15623" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15624" max="15633" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15634" max="15872" width="8.85546875" style="1"/>
     <col min="15873" max="15873" width="4" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="15.6640625" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="25.6640625" style="1" customWidth="1"/>
-    <col min="15876" max="15879" width="14.6640625" style="1" customWidth="1"/>
-    <col min="15880" max="15889" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15890" max="16128" width="8.88671875" style="1"/>
+    <col min="15874" max="15874" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15875" max="15875" width="25.7109375" style="1" customWidth="1"/>
+    <col min="15876" max="15879" width="14.7109375" style="1" customWidth="1"/>
+    <col min="15880" max="15889" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15890" max="16128" width="8.85546875" style="1"/>
     <col min="16129" max="16129" width="4" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="15.6640625" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="25.6640625" style="1" customWidth="1"/>
-    <col min="16132" max="16135" width="14.6640625" style="1" customWidth="1"/>
-    <col min="16136" max="16145" width="12.6640625" style="1" customWidth="1"/>
-    <col min="16146" max="16384" width="8.88671875" style="1"/>
+    <col min="16130" max="16130" width="15.7109375" style="1" customWidth="1"/>
+    <col min="16131" max="16131" width="25.7109375" style="1" customWidth="1"/>
+    <col min="16132" max="16135" width="14.7109375" style="1" customWidth="1"/>
+    <col min="16136" max="16145" width="12.7109375" style="1" customWidth="1"/>
+    <col min="16146" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3278,7 +3278,7 @@
       <c r="Z1" s="77"/>
       <c r="AA1" s="77"/>
     </row>
-    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -3309,7 +3309,7 @@
       <c r="Z2" s="77"/>
       <c r="AA2" s="77"/>
     </row>
-    <row r="3" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="78"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3340,7 +3340,7 @@
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
     </row>
-    <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="78"/>
       <c r="B4" s="85"/>
       <c r="C4" s="85"/>
@@ -3371,7 +3371,7 @@
       <c r="Z4" s="77"/>
       <c r="AA4" s="77"/>
     </row>
-    <row r="5" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="78"/>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -3402,7 +3402,7 @@
       <c r="Z5" s="77"/>
       <c r="AA5" s="77"/>
     </row>
-    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="78"/>
       <c r="B6" s="85"/>
       <c r="C6" s="85"/>
@@ -3433,7 +3433,7 @@
       <c r="Z6" s="77"/>
       <c r="AA6" s="77"/>
     </row>
-    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="78"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
@@ -3464,7 +3464,7 @@
       <c r="Z7" s="77"/>
       <c r="AA7" s="77"/>
     </row>
-    <row r="8" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="78"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3495,7 +3495,7 @@
       <c r="Z8" s="77"/>
       <c r="AA8" s="77"/>
     </row>
-    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="78"/>
       <c r="B9" s="96"/>
       <c r="C9" s="96"/>
@@ -3524,7 +3524,7 @@
       <c r="Z9" s="77"/>
       <c r="AA9" s="77"/>
     </row>
-    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="38" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="99"/>
       <c r="B10" s="100" t="s">
         <v>0</v>
@@ -3561,7 +3561,7 @@
       <c r="Z10" s="106"/>
       <c r="AA10" s="106"/>
     </row>
-    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="107"/>
       <c r="B11" s="108" t="s">
         <v>0</v>
@@ -3598,7 +3598,7 @@
       <c r="Z11" s="112"/>
       <c r="AA11" s="112"/>
     </row>
-    <row r="12" spans="1:27" s="32" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" s="32" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A12" s="78"/>
       <c r="B12" s="108" t="s">
         <v>0</v>
@@ -3635,7 +3635,7 @@
       <c r="Z12" s="84"/>
       <c r="AA12" s="84"/>
     </row>
-    <row r="13" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="77"/>
       <c r="B13" s="108" t="s">
         <v>0</v>
@@ -3672,7 +3672,7 @@
       <c r="Z13" s="77"/>
       <c r="AA13" s="77"/>
     </row>
-    <row r="14" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="77"/>
       <c r="B14" s="108" t="s">
         <v>0</v>
@@ -3709,7 +3709,7 @@
       <c r="Z14" s="77"/>
       <c r="AA14" s="77"/>
     </row>
-    <row r="15" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="77"/>
       <c r="B15" s="108" t="s">
         <v>0</v>
@@ -3746,7 +3746,7 @@
       <c r="Z15" s="77"/>
       <c r="AA15" s="77"/>
     </row>
-    <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="77"/>
       <c r="B16" s="108" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
       <c r="Z16" s="77"/>
       <c r="AA16" s="77"/>
     </row>
-    <row r="17" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B17" s="108" t="s">
         <v>0</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="108" t="s">
         <v>0</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="108" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="108" t="s">
         <v>0</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="108" t="s">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="108" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="108" t="s">
         <v>0</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="108" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H24" s="123"/>
     </row>
-    <row r="25" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B25" s="108" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="H25" s="123"/>
     </row>
-    <row r="26" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B26" s="108" t="s">
         <v>0</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="108" t="s">
         <v>0</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="108" t="s">
         <v>0</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="108" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="108" t="s">
         <v>0</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="108" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="108" t="s">
         <v>0</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="108" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="108" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="108"/>
       <c r="C35" s="109" t="s">
         <v>89</v>
@@ -4100,7 +4100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="108" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="108" t="s">
         <v>0</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="108" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="108" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="108"/>
       <c r="C40" s="109" t="s">
         <v>90</v>
@@ -4183,7 +4183,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="108" t="s">
         <v>0</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="108" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="108" t="s">
         <v>0</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="108" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B45" s="108" t="s">
         <v>0</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B46" s="108" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B47" s="108" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B48" s="108" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B49" s="108" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B50" s="108" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B51" s="108" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B52" s="108" t="s">
         <v>0</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B53" s="108" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B54" s="108"/>
       <c r="C54" s="109" t="s">
         <v>105</v>
@@ -4419,7 +4419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B55" s="108" t="s">
         <v>0</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="F55" s="110"/>
       <c r="G55" s="111"/>
     </row>
-    <row r="56" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B56" s="108" t="s">
         <v>0</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B57" s="108" t="s">
         <v>0</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="F57" s="110"/>
       <c r="G57" s="111"/>
     </row>
-    <row r="58" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="113"/>
       <c r="C58" s="114"/>
       <c r="D58" s="115"/>
@@ -4473,7 +4473,7 @@
       <c r="F58" s="117"/>
       <c r="G58" s="118"/>
     </row>
-    <row r="59" spans="2:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -4481,7 +4481,7 @@
       <c r="F59" s="77"/>
       <c r="G59" s="77"/>
     </row>
-    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B60" s="77"/>
       <c r="C60" s="77"/>
       <c r="D60" s="77"/>
@@ -4489,7 +4489,7 @@
       <c r="F60" s="77"/>
       <c r="G60" s="77"/>
     </row>
-    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B61" s="77"/>
       <c r="C61" s="77"/>
       <c r="D61" s="77"/>
@@ -4497,7 +4497,7 @@
       <c r="F61" s="77"/>
       <c r="G61" s="77"/>
     </row>
-    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B62" s="77"/>
       <c r="C62" s="77"/>
       <c r="D62" s="77"/>
@@ -4505,7 +4505,7 @@
       <c r="F62" s="77"/>
       <c r="G62" s="77"/>
     </row>
-    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B63" s="77"/>
       <c r="C63" s="77"/>
       <c r="D63" s="119"/>
@@ -4513,7 +4513,7 @@
       <c r="F63" s="119"/>
       <c r="G63" s="77"/>
     </row>
-    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="119"/>
@@ -4521,7 +4521,7 @@
       <c r="F64" s="119"/>
       <c r="G64" s="77"/>
     </row>
-    <row r="65" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B65" s="77"/>
       <c r="C65" s="77"/>
       <c r="D65" s="77"/>
@@ -4529,7 +4529,7 @@
       <c r="F65" s="77"/>
       <c r="G65" s="119"/>
     </row>
-    <row r="66" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B66" s="77"/>
       <c r="C66" s="77"/>
       <c r="D66" s="77"/>
@@ -4537,7 +4537,7 @@
       <c r="F66" s="119"/>
       <c r="G66" s="77"/>
     </row>
-    <row r="67" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B67" s="77"/>
       <c r="C67" s="77"/>
       <c r="D67" s="119"/>
@@ -4545,7 +4545,7 @@
       <c r="F67" s="119"/>
       <c r="G67" s="77"/>
     </row>
-    <row r="68" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B68" s="77"/>
       <c r="C68" s="77"/>
       <c r="D68" s="77"/>

</xml_diff>